<commit_message>
Updated Methanol Folder with corrected Temperatures
</commit_message>
<xml_diff>
--- a/Methanol/Methanol_AVE_MASS_FRAC.xlsx
+++ b/Methanol/Methanol_AVE_MASS_FRAC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Git_Repos\Pool_Fires\Methanol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{24D5E615-9B52-4A95-AAF7-21570B94D3EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{638F6774-3A93-47C6-9986-8107F669C341}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="11055" xr2:uid="{043094B6-4485-45EE-82CA-BED423694A52}"/>
+    <workbookView xWindow="25200" yWindow="-11550" windowWidth="16200" windowHeight="10980" xr2:uid="{043094B6-4485-45EE-82CA-BED423694A52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,40 +610,40 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7.0582636882960265E-2</v>
+        <v>7.5943634049407224E-2</v>
       </c>
       <c r="C2">
-        <v>3.9622433182009541E-3</v>
+        <v>4.219131060181059E-3</v>
       </c>
       <c r="D2">
-        <v>0.11436956951653633</v>
+        <v>0.11461536284168035</v>
       </c>
       <c r="E2">
-        <v>6.2441845493744217E-3</v>
+        <v>6.9090002709211633E-3</v>
       </c>
       <c r="F2">
-        <v>2.0001141056166155E-2</v>
+        <v>2.1785783678512083E-2</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0.31847272343489952</v>
+        <v>0.287732562868526</v>
       </c>
       <c r="I2">
-        <v>0.40588937547805326</v>
+        <v>0.42427863914517178</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>6.6731431702013531E-4</v>
+        <v>7.1339141443824789E-4</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>5.9810811446788896E-2</v>
+        <v>6.3802494671161961E-2</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -666,40 +666,40 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>7.8450635810282249E-2</v>
+        <v>8.3004685819327947E-2</v>
       </c>
       <c r="C3">
-        <v>4.3941321424580664E-3</v>
+        <v>4.613479262540833E-3</v>
       </c>
       <c r="D3">
-        <v>0.12179128134061024</v>
+        <v>0.12930083699642483</v>
       </c>
       <c r="E3">
-        <v>6.8891556798070727E-3</v>
+        <v>7.3423152153845803E-3</v>
       </c>
       <c r="F3">
-        <v>1.8972599937024996E-2</v>
+        <v>1.9997835516329554E-2</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.25323883199490904</v>
+        <v>0.226179314894383</v>
       </c>
       <c r="I3">
-        <v>0.44419132643034409</v>
+        <v>0.45382904297834392</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>7.6877934331399576E-4</v>
+        <v>8.1355483070470942E-4</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>7.1303257321250063E-2</v>
+        <v>7.4918934486560618E-2</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -722,40 +722,40 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>8.9721188827749709E-2</v>
+        <v>9.5229880905198364E-2</v>
       </c>
       <c r="C4">
-        <v>3.3784218717039451E-3</v>
+        <v>3.5492355593062272E-3</v>
       </c>
       <c r="D4">
-        <v>0.11541674863319593</v>
+        <v>0.12321852723611326</v>
       </c>
       <c r="E4">
-        <v>8.5025985161090029E-3</v>
+        <v>9.0806051440410207E-3</v>
       </c>
       <c r="F4">
-        <v>3.9037402578242085E-2</v>
+        <v>4.1455826886504184E-2</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0.13822088502552426</v>
+        <v>9.9510439123667999E-2</v>
       </c>
       <c r="I4">
-        <v>0.54444420429838847</v>
+        <v>0.56269098102888626</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>5.7132369717672747E-4</v>
+        <v>6.0435468852042924E-4</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>6.0707226551909868E-2</v>
+        <v>6.4660149427762326E-2</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -778,40 +778,40 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>9.0097215220002455E-2</v>
+        <v>9.6312507739279588E-2</v>
       </c>
       <c r="C5">
-        <v>2.3680013315857122E-3</v>
+        <v>2.5060546242810615E-3</v>
       </c>
       <c r="D5">
-        <v>0.10968548843021463</v>
+        <v>0.11793103702537136</v>
       </c>
       <c r="E5">
-        <v>9.2638539817236978E-3</v>
+        <v>9.9689018086355219E-3</v>
       </c>
       <c r="F5">
-        <v>5.7558729415109075E-2</v>
+        <v>6.162055808232024E-2</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>9.591976791497793E-2</v>
+        <v>4.8868980519427528E-2</v>
       </c>
       <c r="I5">
-        <v>0.59078942691285186</v>
+        <v>0.61524452862486489</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>3.7601935288725214E-4</v>
+        <v>4.0080177420546672E-4</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>4.3941497440647417E-2</v>
+        <v>4.7146629801614277E-2</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -834,40 +834,40 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>9.2495120824868021E-2</v>
+        <v>9.7556872438494702E-2</v>
       </c>
       <c r="C6">
-        <v>1.1964921985279692E-3</v>
+        <v>1.3095539678176804E-3</v>
       </c>
       <c r="D6">
-        <v>8.5130933504318732E-2</v>
+        <v>9.9742275916372927E-2</v>
       </c>
       <c r="E6">
-        <v>9.8093327365538722E-3</v>
+        <v>1.0404302189858937E-2</v>
       </c>
       <c r="F6">
-        <v>9.1724378119066308E-2</v>
+        <v>9.6624594538377948E-2</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>6.6170461476912745E-2</v>
+        <v>2.5268929829495763E-2</v>
       </c>
       <c r="I6">
-        <v>0.62912002812178902</v>
+        <v>0.6433463342058855</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>1.9415657695177839E-4</v>
+        <v>2.1644459621760089E-4</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>2.4159096441011538E-2</v>
+        <v>2.5530692317478801E-2</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -890,40 +890,40 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>7.6187627558948604E-2</v>
+        <v>8.2299028721604536E-2</v>
       </c>
       <c r="C7">
-        <v>7.1080273329158052E-4</v>
+        <v>8.0540559924903161E-4</v>
       </c>
       <c r="D7">
-        <v>7.6518836507483631E-2</v>
+        <v>8.0770735330052232E-2</v>
       </c>
       <c r="E7">
-        <v>1.0189416473605301E-2</v>
+        <v>1.1181294686439296E-2</v>
       </c>
       <c r="F7">
-        <v>0.10934347704623922</v>
+        <v>0.1171752365211685</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>5.7073219572239736E-2</v>
+        <v>2.9954045284091529E-3</v>
       </c>
       <c r="I7">
-        <v>0.65330229960684538</v>
+        <v>0.68668036373075658</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>1.1588553026096467E-4</v>
+        <v>1.3179098418896262E-4</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>1.6558434971085702E-2</v>
+        <v>1.796073989813185E-2</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -946,40 +946,40 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>5.7161713138229001E-2</v>
+        <v>5.8413052794829778E-2</v>
       </c>
       <c r="C8">
-        <v>9.3913070949207467E-5</v>
+        <v>1.5870375684867312E-4</v>
       </c>
       <c r="D8">
-        <v>3.4034525136929707E-2</v>
+        <v>4.8034117724348957E-2</v>
       </c>
       <c r="E8">
-        <v>1.1486395404684263E-2</v>
+        <v>1.1796185776060016E-2</v>
       </c>
       <c r="F8">
-        <v>0.15307992037331164</v>
+        <v>0.15422841289381825</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>3.1803172224408201E-4</v>
       </c>
       <c r="I8">
-        <v>0.74084005472391878</v>
+        <v>0.72386786315594076</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>2.3188282481681027E-5</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>3.3034781519774049E-3</v>
+        <v>3.1604438934276749E-3</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1002,40 +1002,40 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <v>3.1470439631990886E-2</v>
+        <v>3.9495533522106316E-2</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1.5254335440274658E-2</v>
+        <v>3.269526254054541E-2</v>
       </c>
       <c r="E9">
-        <v>1.1677427299986769E-2</v>
+        <v>1.1855314193272237E-2</v>
       </c>
       <c r="F9">
-        <v>0.18431288014380248</v>
+        <v>0.17995647932240258</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>5.7785961129601892E-4</v>
       </c>
       <c r="I9">
-        <v>0.75691514946303717</v>
+        <v>0.7347829650987584</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>4.4261618007156399E-6</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>3.6976802090799916E-4</v>
+        <v>6.321595498183332E-4</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1058,19 +1058,19 @@
         <v>60</v>
       </c>
       <c r="B10">
-        <v>1.3312275954569479E-2</v>
+        <v>1.4459886264583246E-2</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1.1865009655018815E-2</v>
       </c>
       <c r="E10">
-        <v>1.1727555329760612E-2</v>
+        <v>1.2145176273342695E-2</v>
       </c>
       <c r="F10">
-        <v>0.21136708706466936</v>
+        <v>0.21306943527723599</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.76359308165100048</v>
+        <v>0.74846049252981917</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1202,40 +1202,40 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8.08325549730185E-3</v>
+        <v>9.2050117066182456E-3</v>
       </c>
       <c r="C2">
-        <v>2.6239532953176674E-4</v>
+        <v>3.3609724666102563E-4</v>
       </c>
       <c r="D2">
-        <v>2.2238296575399708E-2</v>
+        <v>2.2979121317208685E-2</v>
       </c>
       <c r="E2">
-        <v>3.861300045106309E-4</v>
+        <v>6.1370432448422418E-4</v>
       </c>
       <c r="F2">
-        <v>1.3759187147339739E-3</v>
+        <v>2.0569928391430204E-3</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>7.7603888148622846E-2</v>
+        <v>7.2536173916128294E-2</v>
       </c>
       <c r="I2">
-        <v>2.5248120740824231E-2</v>
+        <v>2.6771951190910557E-2</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>4.4199887297337561E-5</v>
+        <v>6.2995427529744831E-5</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>3.0587084366010941E-3</v>
+        <v>4.0338204234419686E-3</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1258,40 +1258,40 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>8.4893731601230361E-3</v>
+        <v>1.1204041524548663E-2</v>
       </c>
       <c r="C3">
-        <v>5.5502641390490137E-4</v>
+        <v>6.7687925502405832E-4</v>
       </c>
       <c r="D3">
-        <v>3.1070279515932449E-2</v>
+        <v>3.3499305283460984E-2</v>
       </c>
       <c r="E3">
-        <v>9.9492110550290433E-4</v>
+        <v>1.2097500210485378E-3</v>
       </c>
       <c r="F3">
-        <v>1.1209800196081355E-2</v>
+        <v>1.1758540626339927E-2</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0.12968104375272693</v>
+        <v>0.1177652160048267</v>
       </c>
       <c r="I3">
-        <v>6.2535086470102891E-2</v>
+        <v>6.3857950699712868E-2</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>1.0800929930691565E-4</v>
+        <v>1.3663296247674346E-4</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>8.3265359108436448E-3</v>
+        <v>9.9742287911236752E-3</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1314,40 +1314,40 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>8.8805999542884446E-3</v>
+        <v>1.0224437265368716E-2</v>
       </c>
       <c r="C4">
-        <v>4.4835375211424428E-4</v>
+        <v>5.095689670170224E-4</v>
       </c>
       <c r="D4">
-        <v>3.4148741706262926E-2</v>
+        <v>3.687671521963614E-2</v>
       </c>
       <c r="E4">
-        <v>6.1976351637840006E-4</v>
+        <v>1.0677610586162034E-3</v>
       </c>
       <c r="F4">
-        <v>9.8471789354188186E-3</v>
+        <v>1.0389077804728837E-2</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>3.5443207002860293E-2</v>
+        <v>3.8170275331183827E-2</v>
       </c>
       <c r="I4">
-        <v>3.4926531977354389E-2</v>
+        <v>3.8248577916091514E-2</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>7.2119786007922721E-5</v>
+        <v>7.9536493069314116E-5</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>6.8340824973586499E-3</v>
+        <v>7.7613996789671173E-3</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1370,40 +1370,40 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>5.023921377232423E-3</v>
+        <v>5.2019544803832947E-3</v>
       </c>
       <c r="C5">
-        <v>2.8443090352907378E-4</v>
+        <v>3.1704651892104342E-4</v>
       </c>
       <c r="D5">
-        <v>2.5953662408898282E-2</v>
+        <v>2.7956938557151732E-2</v>
       </c>
       <c r="E5">
-        <v>5.0752459484002736E-4</v>
+        <v>9.3528708405208271E-4</v>
       </c>
       <c r="F5">
-        <v>5.9892479584392078E-3</v>
+        <v>6.2542256543869131E-3</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1.8585823475114557E-2</v>
+        <v>1.5915136903460986E-2</v>
       </c>
       <c r="I5">
-        <v>2.9012319505702822E-2</v>
+        <v>2.9060917574679154E-2</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>8.1301067416106619E-5</v>
+        <v>8.7667049512448435E-5</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>3.5180015260110743E-3</v>
+        <v>3.9314019883051167E-3</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1426,40 +1426,40 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>5.3220989985113716E-3</v>
+        <v>6.2220254396788419E-3</v>
       </c>
       <c r="C6">
-        <v>2.7902556816813978E-4</v>
+        <v>3.5719583796350293E-4</v>
       </c>
       <c r="D6">
-        <v>2.100544389444834E-2</v>
+        <v>2.7455374002231081E-2</v>
       </c>
       <c r="E6">
-        <v>4.530458395609544E-4</v>
+        <v>8.9376183043998487E-4</v>
       </c>
       <c r="F6">
-        <v>8.4967599795575943E-3</v>
+        <v>9.614610501094906E-3</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1.1971283633433539E-2</v>
+        <v>1.4634778950769102E-2</v>
       </c>
       <c r="I6">
-        <v>2.0335330121681341E-2</v>
+        <v>2.5826827578832583E-2</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>4.3078579681632526E-5</v>
+        <v>6.6019016451554019E-5</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>5.1613848256857825E-3</v>
+        <v>5.8193001581905105E-3</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1482,40 +1482,40 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>5.5922029804803741E-3</v>
+        <v>6.2086006262574911E-3</v>
       </c>
       <c r="C7">
-        <v>6.829922248316746E-5</v>
+        <v>5.7882600176676193E-5</v>
       </c>
       <c r="D7">
-        <v>2.2778094380127761E-2</v>
+        <v>1.9771611650357908E-2</v>
       </c>
       <c r="E7">
-        <v>3.7874885891858734E-4</v>
+        <v>8.3623237068937764E-4</v>
       </c>
       <c r="F7">
-        <v>9.0600667436006692E-3</v>
+        <v>9.3267757297111828E-3</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1.0357019473375643E-2</v>
+        <v>1.0052958459337001E-3</v>
       </c>
       <c r="I7">
-        <v>1.8517553120933065E-2</v>
+        <v>1.8482430287661514E-2</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>1.6916774133111512E-5</v>
+        <v>7.5216538753842362E-6</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>2.1377300725430068E-3</v>
+        <v>2.1012878523818468E-3</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1538,40 +1538,40 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>3.348383122523552E-3</v>
+        <v>2.0521867080031237E-3</v>
       </c>
       <c r="C8">
-        <v>5.7926563825473222E-6</v>
+        <v>1.2272873485124463E-5</v>
       </c>
       <c r="D8">
-        <v>8.5425852904573024E-3</v>
+        <v>9.1907984360299691E-3</v>
       </c>
       <c r="E8">
-        <v>4.3177366486451293E-4</v>
+        <v>8.6480127968323339E-4</v>
       </c>
       <c r="F8">
-        <v>4.0911475452464381E-3</v>
+        <v>4.0252175709759967E-3</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>2.6626694117635953E-4</v>
       </c>
       <c r="I8">
-        <v>2.212224639897039E-2</v>
+        <v>1.7317782005123915E-2</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>3.0873822898442821E-6</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>2.0945261043214361E-4</v>
+        <v>2.2691971644007769E-4</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1594,40 +1594,40 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <v>1.3508171290016021E-2</v>
+        <v>8.9335471994275218E-4</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>2.8950541473977322E-3</v>
+        <v>6.1962150112454028E-3</v>
       </c>
       <c r="E9">
-        <v>3.7936882646553641E-4</v>
+        <v>8.3420555875280821E-4</v>
       </c>
       <c r="F9">
-        <v>1.6629722503589253E-2</v>
+        <v>3.5401875121342271E-3</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>5.9691805208705527E-5</v>
       </c>
       <c r="I9">
-        <v>1.6361197493086971E-2</v>
+        <v>1.4329578028222857E-2</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>2.3025386894147772E-7</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>5.0596921432687091E-4</v>
+        <v>1.3992253335041258E-5</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1650,19 +1650,19 @@
         <v>60</v>
       </c>
       <c r="B10">
-        <v>1.0582033215719802E-3</v>
+        <v>3.1854513254508596E-4</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2.2477631024692001E-3</v>
       </c>
       <c r="E10">
-        <v>4.0291525124031084E-4</v>
+        <v>8.5232713784051716E-4</v>
       </c>
       <c r="F10">
-        <v>4.811195363770302E-3</v>
+        <v>4.0465404584002947E-3</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1671,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1.8151421259810868E-2</v>
+        <v>1.4082130486613919E-2</v>
       </c>
       <c r="J10">
         <v>0</v>

</xml_diff>